<commit_message>
add enter key event
</commit_message>
<xml_diff>
--- a/src/main/resources/voucher_template_28.xlsx
+++ b/src/main/resources/voucher_template_28.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weici\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouqianhao/Projects/nztrip/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15825" windowHeight="8430"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="21020" windowHeight="15300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,15 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -137,7 +145,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -173,14 +181,14 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -232,30 +240,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -692,27 +700,27 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="H2" s="1"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="I3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -720,15 +728,15 @@
         <v>2</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -736,13 +744,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -750,15 +758,15 @@
         <v>6</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -766,15 +774,15 @@
         <v>21</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -782,15 +790,15 @@
         <v>22</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -798,15 +806,15 @@
         <v>8</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -814,15 +822,15 @@
         <v>10</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -830,15 +838,15 @@
         <v>12</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -846,15 +854,15 @@
         <v>14</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -862,15 +870,15 @@
         <v>16</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -878,27 +886,27 @@
         <v>18</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E14:I14"/>
     <mergeCell ref="E5:I5"/>
     <mergeCell ref="E6:I6"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="E12:I12"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="E14:I14"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -913,7 +921,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -926,7 +934,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>